<commit_message>
Added to majors folder
</commit_message>
<xml_diff>
--- a/Majors%2FMinor%2FTrack Progress.xlsx
+++ b/Majors%2FMinor%2FTrack Progress.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5240" yWindow="3040" windowWidth="25600" windowHeight="15520" tabRatio="500"/>
+    <workbookView xWindow="5940" yWindow="980" windowWidth="25360" windowHeight="15280" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="81">
   <si>
     <t>Major</t>
   </si>
@@ -235,6 +235,33 @@
   </si>
   <si>
     <t>4 Western art history classes (will have to ask a professor about these)</t>
+  </si>
+  <si>
+    <t>"at least three courses in a single Asian language at Furman or three non-language Asian Studies courses" I just put all these things as requirements. We can go back later and or the requirements.</t>
+  </si>
+  <si>
+    <t>12 Additional credits of studio arts (where some THA classes count too)</t>
+  </si>
+  <si>
+    <t>May have a requirement satisfied by an FYW</t>
+  </si>
+  <si>
+    <t>MTH - 120 and 145 or MTH 151</t>
+  </si>
+  <si>
+    <t>Has substitutions, including 2 mayX courses subbing for 1 elective</t>
+  </si>
+  <si>
+    <t>Includes a second major for education oriented students</t>
+  </si>
+  <si>
+    <t>The third elective may be satisfied by 1 couse or by 341 and 342 together</t>
+  </si>
+  <si>
+    <t>Block - I just put the 4 classes as required.</t>
+  </si>
+  <si>
+    <t>Includes education major</t>
   </si>
 </sst>
 </file>
@@ -676,10 +703,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D66"/>
+  <dimension ref="A1:F66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -688,7 +715,7 @@
     <col min="2" max="2" width="19.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:6" ht="16">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -699,7 +726,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="16">
+    <row r="2" spans="1:6" ht="16">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -711,7 +738,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:6" ht="16">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -720,13 +747,13 @@
         <v>69</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:6" ht="16">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="13"/>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:6" ht="16">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -738,253 +765,280 @@
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:6" ht="16">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="4"/>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="B6" s="13"/>
+      <c r="C6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="16">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="4"/>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="B7" s="13"/>
+      <c r="C7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="16">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="4"/>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="B8" s="12"/>
+      <c r="C8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="16">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="4"/>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="B9" s="12"/>
+    </row>
+    <row r="10" spans="1:6" ht="16">
       <c r="A10" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="4"/>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="B10" s="12"/>
+      <c r="C10" t="s">
+        <v>75</v>
+      </c>
+      <c r="D10" t="s">
+        <v>76</v>
+      </c>
+      <c r="E10" t="s">
+        <v>77</v>
+      </c>
+      <c r="F10" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="16">
       <c r="A11" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="4"/>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="B11" s="12"/>
+      <c r="C11" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="16">
       <c r="A12" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="4"/>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="B12" s="12"/>
+      <c r="C12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="16">
       <c r="A13" s="6" t="s">
         <v>14</v>
       </c>
       <c r="B13" s="4"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:6" ht="16">
       <c r="A14" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B14" s="4"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:6" ht="16">
       <c r="A15" s="6" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="4"/>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:6" ht="16">
       <c r="A16" s="5" t="s">
         <v>17</v>
       </c>
       <c r="B16" s="4"/>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" ht="16">
       <c r="A17" s="5" t="s">
         <v>18</v>
       </c>
       <c r="B17" s="4"/>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" ht="16">
       <c r="A18" s="5" t="s">
         <v>19</v>
       </c>
       <c r="B18" s="4"/>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" ht="16">
       <c r="A19" s="5" t="s">
         <v>20</v>
       </c>
       <c r="B19" s="4"/>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" ht="16">
       <c r="A20" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B20" s="4"/>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" ht="16">
       <c r="A21" s="5" t="s">
         <v>22</v>
       </c>
       <c r="B21" s="4"/>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" ht="16">
       <c r="A22" s="5" t="s">
         <v>23</v>
       </c>
       <c r="B22" s="4"/>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" ht="16">
       <c r="A23" s="5" t="s">
         <v>24</v>
       </c>
       <c r="B23" s="4"/>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" ht="16">
       <c r="A24" s="5" t="s">
         <v>25</v>
       </c>
       <c r="B24" s="4"/>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" ht="16">
       <c r="A25" s="5" t="s">
         <v>26</v>
       </c>
       <c r="B25" s="4"/>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" ht="16">
       <c r="A26" s="6" t="s">
         <v>27</v>
       </c>
       <c r="B26" s="4"/>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" ht="16">
       <c r="A27" s="6" t="s">
         <v>28</v>
       </c>
       <c r="B27" s="4"/>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" ht="16">
       <c r="A28" s="6" t="s">
         <v>29</v>
       </c>
       <c r="B28" s="4"/>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" ht="16">
       <c r="A29" s="5" t="s">
         <v>30</v>
       </c>
       <c r="B29" s="4"/>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" ht="16">
       <c r="A30" s="5" t="s">
         <v>31</v>
       </c>
       <c r="B30" s="4"/>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" ht="16">
       <c r="A31" s="6" t="s">
         <v>32</v>
       </c>
       <c r="B31" s="4"/>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" ht="16">
       <c r="A32" s="6" t="s">
         <v>33</v>
       </c>
       <c r="B32" s="4"/>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" ht="16">
       <c r="A33" s="7" t="s">
         <v>34</v>
       </c>
       <c r="B33" s="4"/>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" ht="16">
       <c r="A34" s="7" t="s">
         <v>35</v>
       </c>
       <c r="B34" s="4"/>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" ht="16">
       <c r="A35" s="7" t="s">
         <v>36</v>
       </c>
       <c r="B35" s="4"/>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" ht="16">
       <c r="A36" s="5" t="s">
         <v>37</v>
       </c>
       <c r="B36" s="4"/>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" ht="16">
       <c r="A37" s="5" t="s">
         <v>38</v>
       </c>
       <c r="B37" s="4"/>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" ht="16">
       <c r="A38" s="5" t="s">
         <v>39</v>
       </c>
       <c r="B38" s="4"/>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" ht="16">
       <c r="A39" s="5" t="s">
         <v>40</v>
       </c>
       <c r="B39" s="4"/>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" ht="16">
       <c r="A40" s="5" t="s">
         <v>41</v>
       </c>
       <c r="B40" s="4"/>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" ht="16">
       <c r="A41" s="5" t="s">
         <v>42</v>
       </c>
       <c r="B41" s="4"/>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:2" ht="16">
       <c r="A42" s="5" t="s">
         <v>43</v>
       </c>
       <c r="B42" s="4"/>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:2" ht="16">
       <c r="A43" s="5" t="s">
         <v>44</v>
       </c>
       <c r="B43" s="4"/>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:2" ht="16">
       <c r="A44" s="5" t="s">
         <v>45</v>
       </c>
       <c r="B44" s="4"/>
     </row>
-    <row r="45" spans="1:2">
+    <row r="45" spans="1:2" ht="16">
       <c r="A45" s="5" t="s">
         <v>46</v>
       </c>
       <c r="B45" s="4"/>
     </row>
-    <row r="46" spans="1:2">
+    <row r="46" spans="1:2" ht="16">
       <c r="A46" s="5" t="s">
         <v>47</v>
       </c>
       <c r="B46" s="4"/>
     </row>
-    <row r="47" spans="1:2">
+    <row r="47" spans="1:2" ht="16">
       <c r="A47" s="5" t="s">
         <v>48</v>
       </c>
@@ -996,79 +1050,79 @@
       </c>
       <c r="B48" s="4"/>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" spans="1:2" ht="16">
       <c r="A49" s="5" t="s">
         <v>50</v>
       </c>
       <c r="B49" s="4"/>
     </row>
-    <row r="50" spans="1:2">
+    <row r="50" spans="1:2" ht="16">
       <c r="A50" s="5" t="s">
         <v>51</v>
       </c>
       <c r="B50" s="4"/>
     </row>
-    <row r="51" spans="1:2">
+    <row r="51" spans="1:2" ht="16">
       <c r="A51" s="9" t="s">
         <v>52</v>
       </c>
       <c r="B51" s="4"/>
     </row>
-    <row r="52" spans="1:2">
+    <row r="52" spans="1:2" ht="16">
       <c r="A52" s="9" t="s">
         <v>53</v>
       </c>
       <c r="B52" s="4"/>
     </row>
-    <row r="53" spans="1:2">
+    <row r="53" spans="1:2" ht="16">
       <c r="A53" s="9" t="s">
         <v>54</v>
       </c>
       <c r="B53" s="4"/>
     </row>
-    <row r="54" spans="1:2">
+    <row r="54" spans="1:2" ht="16">
       <c r="A54" s="9" t="s">
         <v>55</v>
       </c>
       <c r="B54" s="4"/>
     </row>
-    <row r="55" spans="1:2">
+    <row r="55" spans="1:2" ht="16">
       <c r="A55" s="9" t="s">
         <v>56</v>
       </c>
       <c r="B55" s="4"/>
     </row>
-    <row r="56" spans="1:2">
+    <row r="56" spans="1:2" ht="16">
       <c r="A56" s="9" t="s">
         <v>57</v>
       </c>
       <c r="B56" s="4"/>
     </row>
-    <row r="57" spans="1:2">
+    <row r="57" spans="1:2" ht="16">
       <c r="A57" s="9" t="s">
         <v>58</v>
       </c>
       <c r="B57" s="4"/>
     </row>
-    <row r="58" spans="1:2">
+    <row r="58" spans="1:2" ht="16">
       <c r="A58" s="9" t="s">
         <v>59</v>
       </c>
       <c r="B58" s="4"/>
     </row>
-    <row r="59" spans="1:2">
+    <row r="59" spans="1:2" ht="16">
       <c r="A59" s="9" t="s">
         <v>60</v>
       </c>
       <c r="B59" s="4"/>
     </row>
-    <row r="60" spans="1:2">
+    <row r="60" spans="1:2" ht="16">
       <c r="A60" s="9" t="s">
         <v>61</v>
       </c>
       <c r="B60" s="4"/>
     </row>
-    <row r="61" spans="1:2">
+    <row r="61" spans="1:2" ht="16">
       <c r="A61" s="9" t="s">
         <v>61</v>
       </c>
@@ -1080,25 +1134,25 @@
       </c>
       <c r="B62" s="4"/>
     </row>
-    <row r="63" spans="1:2">
+    <row r="63" spans="1:2" ht="16">
       <c r="A63" s="3" t="s">
         <v>63</v>
       </c>
       <c r="B63" s="4"/>
     </row>
-    <row r="64" spans="1:2">
+    <row r="64" spans="1:2" ht="16">
       <c r="A64" s="3" t="s">
         <v>64</v>
       </c>
       <c r="B64" s="4"/>
     </row>
-    <row r="65" spans="1:2">
+    <row r="65" spans="1:2" ht="16">
       <c r="A65" s="3" t="s">
         <v>65</v>
       </c>
       <c r="B65" s="4"/>
     </row>
-    <row r="66" spans="1:2">
+    <row r="66" spans="1:2" ht="16">
       <c r="A66" s="3" t="s">
         <v>66</v>
       </c>

</xml_diff>